<commit_message>
bo cuc giao dien
</commit_message>
<xml_diff>
--- a/backup/file tạm/qt7.xlsx
+++ b/backup/file tạm/qt7.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My PC HOME\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My PC HOME\code\backup\file tạm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Tên quy trình:</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Đến Form 3</t>
+  </si>
+  <si>
+    <t>1.010724.000.00.00.H13-1</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,7 +497,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -606,6 +609,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>